<commit_message>
14.11.23 Snake game Game Engine Complete
</commit_message>
<xml_diff>
--- a/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
+++ b/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
   <si>
     <t>Classe :</t>
   </si>
@@ -212,6 +212,48 @@
   </si>
   <si>
     <t xml:space="preserve"> Chier de charge et présentation du projet</t>
+  </si>
+  <si>
+    <t>Installation de logiciels : Teams, One Drive et Visual Code</t>
+  </si>
+  <si>
+    <t>Création de JNLTRAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction de la page de garde du document, du style et de la typographie, des pieds de page et de la structure de l’index.  Principes de base de JavasScript terminés </t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>Création de le rapport github et installation de Github sur le PC</t>
+  </si>
+  <si>
+    <t>https://github.com/Adrtoledocam/P_Bulles_Snake</t>
+  </si>
+  <si>
+    <t>Mis a jour de le JNLTRAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contenu de base sur le javascript, ses fondamentaux, les données, les objets, les boucles, les fonctions, les tableaux et les interactions en espagnol. </t>
+  </si>
+  <si>
+    <t>https://javascript.info/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://javascript.info/ </t>
+  </si>
+  <si>
+    <t>Recherche d'information</t>
+  </si>
+  <si>
+    <t>Recherche d'exemples de fonctionnement du canvas et de la théorie du jeu du serpent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.section.io/engineering-education/how-to-build-a-snake-game-with-javascript/ </t>
+  </si>
+  <si>
+    <t>Code: Création de l'arrière-plan, création de canvas, division de canvas, création du score, création de la nourriture, création du serpent (seule la tête interagit, pas de collision pour le corps), fonctions GameOver, Draw et Update (GameEngine). Création d'imputs (erreurs pour se déplacer à l'intérieur du corps).</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1077,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1309,6 +1351,10 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1338,7 +1384,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1406,7 +1456,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
@@ -1464,7 +1514,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -1522,9 +1572,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>114300</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1585,9 +1635,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1648,9 +1698,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1994,7 +2044,7 @@
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2210,10 +2260,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="112" t="s">
+      <c r="B19" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="113"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -2367,7 +2417,9 @@
       <c r="B31" s="80">
         <v>11</v>
       </c>
-      <c r="C31" s="71"/>
+      <c r="C31" s="71" t="s">
+        <v>51</v>
+      </c>
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
       <c r="F31" s="60"/>
@@ -2384,7 +2436,9 @@
       <c r="B32" s="82">
         <v>12</v>
       </c>
-      <c r="C32" s="71"/>
+      <c r="C32" s="71" t="s">
+        <v>58</v>
+      </c>
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
       <c r="F32" s="60"/>
@@ -3055,27 +3109,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3105,27 +3159,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3161,146 +3215,146 @@
       <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="114" t="s">
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="115"/>
-      <c r="AF2" s="115"/>
-      <c r="AG2" s="116"/>
-      <c r="AH2" s="114" t="s">
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="117"/>
+      <c r="AH2" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="115"/>
-      <c r="AM2" s="115"/>
-      <c r="AN2" s="115"/>
-      <c r="AO2" s="115"/>
-      <c r="AP2" s="115"/>
-      <c r="AQ2" s="115"/>
-      <c r="AR2" s="115"/>
-      <c r="AS2" s="115"/>
-      <c r="AT2" s="115"/>
-      <c r="AU2" s="115"/>
-      <c r="AV2" s="116"/>
-      <c r="AW2" s="114" t="s">
+      <c r="AI2" s="116"/>
+      <c r="AJ2" s="116"/>
+      <c r="AK2" s="116"/>
+      <c r="AL2" s="116"/>
+      <c r="AM2" s="116"/>
+      <c r="AN2" s="116"/>
+      <c r="AO2" s="116"/>
+      <c r="AP2" s="116"/>
+      <c r="AQ2" s="116"/>
+      <c r="AR2" s="116"/>
+      <c r="AS2" s="116"/>
+      <c r="AT2" s="116"/>
+      <c r="AU2" s="116"/>
+      <c r="AV2" s="117"/>
+      <c r="AW2" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="115"/>
-      <c r="AY2" s="115"/>
-      <c r="AZ2" s="115"/>
-      <c r="BA2" s="115"/>
-      <c r="BB2" s="115"/>
-      <c r="BC2" s="115"/>
-      <c r="BD2" s="115"/>
-      <c r="BE2" s="115"/>
-      <c r="BF2" s="115"/>
-      <c r="BG2" s="115"/>
-      <c r="BH2" s="115"/>
-      <c r="BI2" s="115"/>
-      <c r="BJ2" s="115"/>
-      <c r="BK2" s="116"/>
-      <c r="BL2" s="114" t="s">
+      <c r="AX2" s="116"/>
+      <c r="AY2" s="116"/>
+      <c r="AZ2" s="116"/>
+      <c r="BA2" s="116"/>
+      <c r="BB2" s="116"/>
+      <c r="BC2" s="116"/>
+      <c r="BD2" s="116"/>
+      <c r="BE2" s="116"/>
+      <c r="BF2" s="116"/>
+      <c r="BG2" s="116"/>
+      <c r="BH2" s="116"/>
+      <c r="BI2" s="116"/>
+      <c r="BJ2" s="116"/>
+      <c r="BK2" s="117"/>
+      <c r="BL2" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="BM2" s="115"/>
-      <c r="BN2" s="115"/>
-      <c r="BO2" s="115"/>
-      <c r="BP2" s="115"/>
-      <c r="BQ2" s="115"/>
-      <c r="BR2" s="115"/>
-      <c r="BS2" s="115"/>
-      <c r="BT2" s="115"/>
-      <c r="BU2" s="115"/>
-      <c r="BV2" s="115"/>
-      <c r="BW2" s="115"/>
-      <c r="BX2" s="115"/>
-      <c r="BY2" s="115"/>
-      <c r="BZ2" s="116"/>
-      <c r="CA2" s="114" t="s">
+      <c r="BM2" s="116"/>
+      <c r="BN2" s="116"/>
+      <c r="BO2" s="116"/>
+      <c r="BP2" s="116"/>
+      <c r="BQ2" s="116"/>
+      <c r="BR2" s="116"/>
+      <c r="BS2" s="116"/>
+      <c r="BT2" s="116"/>
+      <c r="BU2" s="116"/>
+      <c r="BV2" s="116"/>
+      <c r="BW2" s="116"/>
+      <c r="BX2" s="116"/>
+      <c r="BY2" s="116"/>
+      <c r="BZ2" s="117"/>
+      <c r="CA2" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="CB2" s="115"/>
-      <c r="CC2" s="115"/>
-      <c r="CD2" s="115"/>
-      <c r="CE2" s="115"/>
-      <c r="CF2" s="115"/>
-      <c r="CG2" s="115"/>
-      <c r="CH2" s="115"/>
-      <c r="CI2" s="115"/>
-      <c r="CJ2" s="115"/>
-      <c r="CK2" s="115"/>
-      <c r="CL2" s="115"/>
-      <c r="CM2" s="115"/>
-      <c r="CN2" s="115"/>
-      <c r="CO2" s="116"/>
-      <c r="CP2" s="114" t="s">
+      <c r="CB2" s="116"/>
+      <c r="CC2" s="116"/>
+      <c r="CD2" s="116"/>
+      <c r="CE2" s="116"/>
+      <c r="CF2" s="116"/>
+      <c r="CG2" s="116"/>
+      <c r="CH2" s="116"/>
+      <c r="CI2" s="116"/>
+      <c r="CJ2" s="116"/>
+      <c r="CK2" s="116"/>
+      <c r="CL2" s="116"/>
+      <c r="CM2" s="116"/>
+      <c r="CN2" s="116"/>
+      <c r="CO2" s="117"/>
+      <c r="CP2" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="CQ2" s="115"/>
-      <c r="CR2" s="115"/>
-      <c r="CS2" s="115"/>
-      <c r="CT2" s="115"/>
-      <c r="CU2" s="115"/>
-      <c r="CV2" s="115"/>
-      <c r="CW2" s="115"/>
-      <c r="CX2" s="115"/>
-      <c r="CY2" s="115"/>
-      <c r="CZ2" s="115"/>
-      <c r="DA2" s="115"/>
-      <c r="DB2" s="115"/>
-      <c r="DC2" s="115"/>
-      <c r="DD2" s="116"/>
-      <c r="DE2" s="114" t="s">
+      <c r="CQ2" s="116"/>
+      <c r="CR2" s="116"/>
+      <c r="CS2" s="116"/>
+      <c r="CT2" s="116"/>
+      <c r="CU2" s="116"/>
+      <c r="CV2" s="116"/>
+      <c r="CW2" s="116"/>
+      <c r="CX2" s="116"/>
+      <c r="CY2" s="116"/>
+      <c r="CZ2" s="116"/>
+      <c r="DA2" s="116"/>
+      <c r="DB2" s="116"/>
+      <c r="DC2" s="116"/>
+      <c r="DD2" s="117"/>
+      <c r="DE2" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="DF2" s="115"/>
-      <c r="DG2" s="115"/>
-      <c r="DH2" s="115"/>
-      <c r="DI2" s="115"/>
-      <c r="DJ2" s="115"/>
-      <c r="DK2" s="115"/>
-      <c r="DL2" s="115"/>
-      <c r="DM2" s="115"/>
-      <c r="DN2" s="115"/>
-      <c r="DO2" s="115"/>
-      <c r="DP2" s="115"/>
-      <c r="DQ2" s="115"/>
-      <c r="DR2" s="115"/>
-      <c r="DS2" s="116"/>
+      <c r="DF2" s="116"/>
+      <c r="DG2" s="116"/>
+      <c r="DH2" s="116"/>
+      <c r="DI2" s="116"/>
+      <c r="DJ2" s="116"/>
+      <c r="DK2" s="116"/>
+      <c r="DL2" s="116"/>
+      <c r="DM2" s="116"/>
+      <c r="DN2" s="116"/>
+      <c r="DO2" s="116"/>
+      <c r="DP2" s="116"/>
+      <c r="DQ2" s="116"/>
+      <c r="DR2" s="116"/>
+      <c r="DS2" s="117"/>
     </row>
     <row r="3" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90"/>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="120" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="16">
@@ -3429,7 +3483,7 @@
     </row>
     <row r="4" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="90"/>
-      <c r="B4" s="120"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3555,7 +3609,7 @@
       <c r="DS4" s="100"/>
     </row>
     <row r="5" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="121" t="str">
+      <c r="B5" s="122" t="str">
         <f>Donnees!$C$21</f>
         <v>Rédaction JNLTRAV</v>
       </c>
@@ -3684,7 +3738,7 @@
       <c r="DS5" s="95"/>
     </row>
     <row r="6" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="118"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="102">
         <v>0</v>
       </c>
@@ -3810,7 +3864,7 @@
       <c r="DS6" s="100"/>
     </row>
     <row r="7" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="117" t="str">
+      <c r="B7" s="118" t="str">
         <f>Donnees!$C$22</f>
         <v>Vacances</v>
       </c>
@@ -3939,7 +3993,7 @@
       <c r="DS7" s="95"/>
     </row>
     <row r="8" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="118"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="102">
         <v>0</v>
       </c>
@@ -4065,7 +4119,7 @@
       <c r="DS8" s="100"/>
     </row>
     <row r="9" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="117" t="str">
+      <c r="B9" s="118" t="str">
         <f>Donnees!$C$23</f>
         <v>Absent</v>
       </c>
@@ -4194,7 +4248,7 @@
       <c r="DS9" s="95"/>
     </row>
     <row r="10" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="118"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="102">
         <v>0</v>
       </c>
@@ -4320,7 +4374,7 @@
       <c r="DS10" s="100"/>
     </row>
     <row r="11" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="117" t="str">
+      <c r="B11" s="118" t="str">
         <f>Donnees!$C$24</f>
         <v>Autres</v>
       </c>
@@ -4449,7 +4503,7 @@
       <c r="DS11" s="95"/>
     </row>
     <row r="12" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="118"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="102">
         <v>0</v>
       </c>
@@ -4575,7 +4629,7 @@
       <c r="DS12" s="100"/>
     </row>
     <row r="13" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="117" t="str">
+      <c r="B13" s="118" t="str">
         <f>Donnees!$C$25</f>
         <v>P_B : code</v>
       </c>
@@ -4704,7 +4758,7 @@
       <c r="DS13" s="95"/>
     </row>
     <row r="14" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="118"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="102">
         <v>0</v>
       </c>
@@ -4830,7 +4884,7 @@
       <c r="DS14" s="100"/>
     </row>
     <row r="15" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="117" t="str">
+      <c r="B15" s="118" t="str">
         <f>Donnees!$C$26</f>
         <v xml:space="preserve">P_B : support de cours </v>
       </c>
@@ -4960,7 +5014,7 @@
     </row>
     <row r="16" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="103"/>
-      <c r="B16" s="118"/>
+      <c r="B16" s="119"/>
       <c r="C16" s="102">
         <v>0</v>
       </c>
@@ -5086,7 +5140,7 @@
       <c r="DS16" s="100"/>
     </row>
     <row r="17" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="117" t="str">
+      <c r="B17" s="118" t="str">
         <f>Donnees!$C$27</f>
         <v>Livraison</v>
       </c>
@@ -5215,7 +5269,7 @@
       <c r="DS17" s="95"/>
     </row>
     <row r="18" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="118"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="102">
         <v>0</v>
       </c>
@@ -5341,7 +5395,7 @@
       <c r="DS18" s="100"/>
     </row>
     <row r="19" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="117" t="str">
+      <c r="B19" s="118" t="str">
         <f>Donnees!$C$28</f>
         <v>JavaScriptInfo</v>
       </c>
@@ -5470,7 +5524,7 @@
       <c r="DS19" s="95"/>
     </row>
     <row r="20" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="118"/>
+      <c r="B20" s="119"/>
       <c r="C20" s="102">
         <v>0</v>
       </c>
@@ -5596,7 +5650,7 @@
       <c r="DS20" s="100"/>
     </row>
     <row r="21" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="117" t="str">
+      <c r="B21" s="118" t="str">
         <f>Donnees!$C$29</f>
         <v>Test</v>
       </c>
@@ -5725,7 +5779,7 @@
       <c r="DS21" s="95"/>
     </row>
     <row r="22" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="118"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="102">
         <v>0</v>
       </c>
@@ -5851,7 +5905,7 @@
       <c r="DS22" s="100"/>
     </row>
     <row r="23" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="117" t="str">
+      <c r="B23" s="118" t="str">
         <f>Donnees!$C$30</f>
         <v>Présentation du corus</v>
       </c>
@@ -5980,7 +6034,7 @@
       <c r="DS23" s="95"/>
     </row>
     <row r="24" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="118"/>
+      <c r="B24" s="119"/>
       <c r="C24" s="102">
         <v>0</v>
       </c>
@@ -6366,6 +6420,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D2:R2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="DE2:DS2"/>
     <mergeCell ref="S2:AG2"/>
     <mergeCell ref="AH2:AV2"/>
@@ -6373,18 +6439,6 @@
     <mergeCell ref="BL2:BZ2"/>
     <mergeCell ref="CA2:CO2"/>
     <mergeCell ref="CP2:DD2"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D2:R2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C25">
@@ -6428,7 +6482,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="120" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="16">
@@ -6437,7 +6491,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="122"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -7241,7 +7295,7 @@
   <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7289,34 +7343,62 @@
       <c r="B3" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="112" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+    <row r="4" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="125" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="124" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="125" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -7384,7 +7466,7 @@
       </c>
       <c r="B18" s="48">
         <f>SUM(B3:B17)</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C18" s="111" t="s">
         <v>45</v>
@@ -7427,21 +7509,39 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="112" t="s">
+        <v>54</v>
+      </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+    <row r="23" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
+      <c r="C23" s="124" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="125" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="124" t="s">
+        <v>61</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -7450,10 +7550,18 @@
       <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="124" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="125" t="s">
+        <v>60</v>
+      </c>
       <c r="E25" s="20"/>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -7587,7 +7695,7 @@
       </c>
       <c r="B37" s="48">
         <f>SUM(B22:B36)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C37" s="111" t="s">
         <v>45</v>
@@ -8466,15 +8574,21 @@
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D23" r:id="rId3"/>
+    <hyperlink ref="D25" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="48129" r:id="rId4" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="48129" r:id="rId8" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -8493,7 +8607,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="48129" r:id="rId4" name="btnImportRealisation"/>
+        <control shapeId="48129" r:id="rId8" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8501,26 +8615,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4cb0ad740d14d835234d40feeeca33f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8afc1019b1abb7dd8f9636ee686097" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -8737,7 +8831,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F035731F-8448-43E0-A923-EE7485D1B78B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25576F2-DA56-4DAD-9B77-0093008FA3D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8754,31 +8895,4 @@
     <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F035731F-8448-43E0-A923-EE7485D1B78B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
-    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update du code du JS et CSS
Correction de la position des éléments en fonction de la taille de l'écran.
Recréation du code sans utiliser les boucles while et for
Fonctionnement en mode pause
</commit_message>
<xml_diff>
--- a/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
+++ b/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrtoledoca\Documents\GitHub\P_Bulles_Snake\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrtoledoca\OneDrive - Education Vaud\ETML\CID2B\2\P_Bulles\P_Bulles_Snake\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
   <si>
     <t>Classe :</t>
   </si>
@@ -261,6 +261,29 @@
 Possibilité de rejouer le jeu
 Mode pause (non terminé)
 Fruits correctement positionnés sur la carte</t>
+  </si>
+  <si>
+    <t>Correction du menu
+Correction de la position du texte sur l'écran.
+Sélection de la police 
+Créer un fond et le recadrer en png 
+Création de boutons 
+Actions des boutons pour permettre de les déplacer dans le jeu par des clics de souris</t>
+  </si>
+  <si>
+    <t>Recherche d'images pour le background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment utiliser la trame d'animation en java </t>
+  </si>
+  <si>
+    <t>Organisation des dossiers dans github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction de la position des éléments en fonction de la taille de l'écran.
+Recréation du code sans utiliser les boucles while et for 
+Fonctionnement en mode pause 
+</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1107,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1376,12 +1399,6 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1391,6 +1408,12 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1399,6 +1422,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3116,27 +3143,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3166,27 +3193,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3222,142 +3249,142 @@
       <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="121"/>
-      <c r="S2" s="119" t="s">
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="120"/>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="120"/>
-      <c r="AE2" s="120"/>
-      <c r="AF2" s="120"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="119" t="s">
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+      <c r="AA2" s="118"/>
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="118"/>
+      <c r="AD2" s="118"/>
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="118"/>
+      <c r="AG2" s="119"/>
+      <c r="AH2" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="120"/>
-      <c r="AJ2" s="120"/>
-      <c r="AK2" s="120"/>
-      <c r="AL2" s="120"/>
-      <c r="AM2" s="120"/>
-      <c r="AN2" s="120"/>
-      <c r="AO2" s="120"/>
-      <c r="AP2" s="120"/>
-      <c r="AQ2" s="120"/>
-      <c r="AR2" s="120"/>
-      <c r="AS2" s="120"/>
-      <c r="AT2" s="120"/>
-      <c r="AU2" s="120"/>
-      <c r="AV2" s="121"/>
-      <c r="AW2" s="119" t="s">
+      <c r="AI2" s="118"/>
+      <c r="AJ2" s="118"/>
+      <c r="AK2" s="118"/>
+      <c r="AL2" s="118"/>
+      <c r="AM2" s="118"/>
+      <c r="AN2" s="118"/>
+      <c r="AO2" s="118"/>
+      <c r="AP2" s="118"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="118"/>
+      <c r="AS2" s="118"/>
+      <c r="AT2" s="118"/>
+      <c r="AU2" s="118"/>
+      <c r="AV2" s="119"/>
+      <c r="AW2" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="120"/>
-      <c r="AY2" s="120"/>
-      <c r="AZ2" s="120"/>
-      <c r="BA2" s="120"/>
-      <c r="BB2" s="120"/>
-      <c r="BC2" s="120"/>
-      <c r="BD2" s="120"/>
-      <c r="BE2" s="120"/>
-      <c r="BF2" s="120"/>
-      <c r="BG2" s="120"/>
-      <c r="BH2" s="120"/>
-      <c r="BI2" s="120"/>
-      <c r="BJ2" s="120"/>
-      <c r="BK2" s="121"/>
-      <c r="BL2" s="119" t="s">
+      <c r="AX2" s="118"/>
+      <c r="AY2" s="118"/>
+      <c r="AZ2" s="118"/>
+      <c r="BA2" s="118"/>
+      <c r="BB2" s="118"/>
+      <c r="BC2" s="118"/>
+      <c r="BD2" s="118"/>
+      <c r="BE2" s="118"/>
+      <c r="BF2" s="118"/>
+      <c r="BG2" s="118"/>
+      <c r="BH2" s="118"/>
+      <c r="BI2" s="118"/>
+      <c r="BJ2" s="118"/>
+      <c r="BK2" s="119"/>
+      <c r="BL2" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="BM2" s="120"/>
-      <c r="BN2" s="120"/>
-      <c r="BO2" s="120"/>
-      <c r="BP2" s="120"/>
-      <c r="BQ2" s="120"/>
-      <c r="BR2" s="120"/>
-      <c r="BS2" s="120"/>
-      <c r="BT2" s="120"/>
-      <c r="BU2" s="120"/>
-      <c r="BV2" s="120"/>
-      <c r="BW2" s="120"/>
-      <c r="BX2" s="120"/>
-      <c r="BY2" s="120"/>
-      <c r="BZ2" s="121"/>
-      <c r="CA2" s="119" t="s">
+      <c r="BM2" s="118"/>
+      <c r="BN2" s="118"/>
+      <c r="BO2" s="118"/>
+      <c r="BP2" s="118"/>
+      <c r="BQ2" s="118"/>
+      <c r="BR2" s="118"/>
+      <c r="BS2" s="118"/>
+      <c r="BT2" s="118"/>
+      <c r="BU2" s="118"/>
+      <c r="BV2" s="118"/>
+      <c r="BW2" s="118"/>
+      <c r="BX2" s="118"/>
+      <c r="BY2" s="118"/>
+      <c r="BZ2" s="119"/>
+      <c r="CA2" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="CB2" s="120"/>
-      <c r="CC2" s="120"/>
-      <c r="CD2" s="120"/>
-      <c r="CE2" s="120"/>
-      <c r="CF2" s="120"/>
-      <c r="CG2" s="120"/>
-      <c r="CH2" s="120"/>
-      <c r="CI2" s="120"/>
-      <c r="CJ2" s="120"/>
-      <c r="CK2" s="120"/>
-      <c r="CL2" s="120"/>
-      <c r="CM2" s="120"/>
-      <c r="CN2" s="120"/>
-      <c r="CO2" s="121"/>
-      <c r="CP2" s="119" t="s">
+      <c r="CB2" s="118"/>
+      <c r="CC2" s="118"/>
+      <c r="CD2" s="118"/>
+      <c r="CE2" s="118"/>
+      <c r="CF2" s="118"/>
+      <c r="CG2" s="118"/>
+      <c r="CH2" s="118"/>
+      <c r="CI2" s="118"/>
+      <c r="CJ2" s="118"/>
+      <c r="CK2" s="118"/>
+      <c r="CL2" s="118"/>
+      <c r="CM2" s="118"/>
+      <c r="CN2" s="118"/>
+      <c r="CO2" s="119"/>
+      <c r="CP2" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="CQ2" s="120"/>
-      <c r="CR2" s="120"/>
-      <c r="CS2" s="120"/>
-      <c r="CT2" s="120"/>
-      <c r="CU2" s="120"/>
-      <c r="CV2" s="120"/>
-      <c r="CW2" s="120"/>
-      <c r="CX2" s="120"/>
-      <c r="CY2" s="120"/>
-      <c r="CZ2" s="120"/>
-      <c r="DA2" s="120"/>
-      <c r="DB2" s="120"/>
-      <c r="DC2" s="120"/>
-      <c r="DD2" s="121"/>
-      <c r="DE2" s="119" t="s">
+      <c r="CQ2" s="118"/>
+      <c r="CR2" s="118"/>
+      <c r="CS2" s="118"/>
+      <c r="CT2" s="118"/>
+      <c r="CU2" s="118"/>
+      <c r="CV2" s="118"/>
+      <c r="CW2" s="118"/>
+      <c r="CX2" s="118"/>
+      <c r="CY2" s="118"/>
+      <c r="CZ2" s="118"/>
+      <c r="DA2" s="118"/>
+      <c r="DB2" s="118"/>
+      <c r="DC2" s="118"/>
+      <c r="DD2" s="119"/>
+      <c r="DE2" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="DF2" s="120"/>
-      <c r="DG2" s="120"/>
-      <c r="DH2" s="120"/>
-      <c r="DI2" s="120"/>
-      <c r="DJ2" s="120"/>
-      <c r="DK2" s="120"/>
-      <c r="DL2" s="120"/>
-      <c r="DM2" s="120"/>
-      <c r="DN2" s="120"/>
-      <c r="DO2" s="120"/>
-      <c r="DP2" s="120"/>
-      <c r="DQ2" s="120"/>
-      <c r="DR2" s="120"/>
-      <c r="DS2" s="121"/>
+      <c r="DF2" s="118"/>
+      <c r="DG2" s="118"/>
+      <c r="DH2" s="118"/>
+      <c r="DI2" s="118"/>
+      <c r="DJ2" s="118"/>
+      <c r="DK2" s="118"/>
+      <c r="DL2" s="118"/>
+      <c r="DM2" s="118"/>
+      <c r="DN2" s="118"/>
+      <c r="DO2" s="118"/>
+      <c r="DP2" s="118"/>
+      <c r="DQ2" s="118"/>
+      <c r="DR2" s="118"/>
+      <c r="DS2" s="119"/>
     </row>
     <row r="3" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90"/>
@@ -3745,7 +3772,7 @@
       <c r="DS5" s="95"/>
     </row>
     <row r="6" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="118"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="102">
         <v>0</v>
       </c>
@@ -3871,7 +3898,7 @@
       <c r="DS6" s="100"/>
     </row>
     <row r="7" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="117" t="str">
+      <c r="B7" s="120" t="str">
         <f>Donnees!$C$22</f>
         <v>Vacances</v>
       </c>
@@ -4000,7 +4027,7 @@
       <c r="DS7" s="95"/>
     </row>
     <row r="8" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="118"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="102">
         <v>0</v>
       </c>
@@ -4126,7 +4153,7 @@
       <c r="DS8" s="100"/>
     </row>
     <row r="9" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="117" t="str">
+      <c r="B9" s="120" t="str">
         <f>Donnees!$C$23</f>
         <v>Absent</v>
       </c>
@@ -4255,7 +4282,7 @@
       <c r="DS9" s="95"/>
     </row>
     <row r="10" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="118"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="102">
         <v>0</v>
       </c>
@@ -4381,7 +4408,7 @@
       <c r="DS10" s="100"/>
     </row>
     <row r="11" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="117" t="str">
+      <c r="B11" s="120" t="str">
         <f>Donnees!$C$24</f>
         <v>Autres</v>
       </c>
@@ -4510,7 +4537,7 @@
       <c r="DS11" s="95"/>
     </row>
     <row r="12" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="118"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="102">
         <v>0</v>
       </c>
@@ -4636,7 +4663,7 @@
       <c r="DS12" s="100"/>
     </row>
     <row r="13" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="117" t="str">
+      <c r="B13" s="120" t="str">
         <f>Donnees!$C$25</f>
         <v>P_B : code</v>
       </c>
@@ -4765,7 +4792,7 @@
       <c r="DS13" s="95"/>
     </row>
     <row r="14" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="118"/>
+      <c r="B14" s="121"/>
       <c r="C14" s="102">
         <v>0</v>
       </c>
@@ -4891,7 +4918,7 @@
       <c r="DS14" s="100"/>
     </row>
     <row r="15" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="117" t="str">
+      <c r="B15" s="120" t="str">
         <f>Donnees!$C$26</f>
         <v xml:space="preserve">P_B : support de cours </v>
       </c>
@@ -5021,7 +5048,7 @@
     </row>
     <row r="16" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="103"/>
-      <c r="B16" s="118"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="102">
         <v>0</v>
       </c>
@@ -5147,7 +5174,7 @@
       <c r="DS16" s="100"/>
     </row>
     <row r="17" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="117" t="str">
+      <c r="B17" s="120" t="str">
         <f>Donnees!$C$27</f>
         <v>Livraison</v>
       </c>
@@ -5276,7 +5303,7 @@
       <c r="DS17" s="95"/>
     </row>
     <row r="18" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="118"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="102">
         <v>0</v>
       </c>
@@ -5402,7 +5429,7 @@
       <c r="DS18" s="100"/>
     </row>
     <row r="19" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="117" t="str">
+      <c r="B19" s="120" t="str">
         <f>Donnees!$C$28</f>
         <v>JavaScriptInfo</v>
       </c>
@@ -5531,7 +5558,7 @@
       <c r="DS19" s="95"/>
     </row>
     <row r="20" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="118"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="102">
         <v>0</v>
       </c>
@@ -5657,7 +5684,7 @@
       <c r="DS20" s="100"/>
     </row>
     <row r="21" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="117" t="str">
+      <c r="B21" s="120" t="str">
         <f>Donnees!$C$29</f>
         <v>Test</v>
       </c>
@@ -5786,7 +5813,7 @@
       <c r="DS21" s="95"/>
     </row>
     <row r="22" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="118"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="102">
         <v>0</v>
       </c>
@@ -5912,7 +5939,7 @@
       <c r="DS22" s="100"/>
     </row>
     <row r="23" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="117" t="str">
+      <c r="B23" s="120" t="str">
         <f>Donnees!$C$30</f>
         <v>Présentation du corus</v>
       </c>
@@ -6041,7 +6068,7 @@
       <c r="DS23" s="95"/>
     </row>
     <row r="24" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="118"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="102">
         <v>0</v>
       </c>
@@ -6427,6 +6454,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D2:R2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="DE2:DS2"/>
     <mergeCell ref="S2:AG2"/>
     <mergeCell ref="AH2:AV2"/>
@@ -6434,18 +6473,6 @@
     <mergeCell ref="BL2:BZ2"/>
     <mergeCell ref="CA2:CO2"/>
     <mergeCell ref="CP2:DD2"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D2:R2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C25">
@@ -7301,8 +7328,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7773,7 +7800,7 @@
     </row>
     <row r="42" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2">
         <v>14</v>
@@ -7910,21 +7937,39 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="9"/>
+      <c r="A60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+      <c r="C60" s="112" t="s">
+        <v>54</v>
+      </c>
       <c r="D60" s="9"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="10"/>
+    <row r="61" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2</v>
+      </c>
+      <c r="C61" s="113" t="s">
+        <v>63</v>
+      </c>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="10"/>
+    <row r="62" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="2">
+        <v>12</v>
+      </c>
+      <c r="C62" s="113" t="s">
+        <v>62</v>
+      </c>
       <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -8005,7 +8050,7 @@
       </c>
       <c r="B75" s="48">
         <f>SUM(B60:B74)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C75" s="111" t="s">
         <v>45</v>
@@ -8047,28 +8092,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="9"/>
+    <row r="79" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A79" s="126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B79" s="4">
+        <v>10</v>
+      </c>
+      <c r="C79" s="112" t="s">
+        <v>66</v>
+      </c>
       <c r="D79" s="9"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="10"/>
+    <row r="80" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="10"/>
+    <row r="81" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="10"/>
+      <c r="A82" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1</v>
+      </c>
+      <c r="C82" s="112" t="s">
+        <v>54</v>
+      </c>
       <c r="D82" s="10"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -8143,7 +8212,7 @@
       </c>
       <c r="B94" s="48">
         <f>SUM(B79:B93)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C94" s="111" t="s">
         <v>45</v>
@@ -8633,26 +8702,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4cb0ad740d14d835234d40feeeca33f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8afc1019b1abb7dd8f9636ee686097" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -8869,34 +8918,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25576F2-DA56-4DAD-9B77-0093008FA3D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="15a2adb2-9a92-45bc-9379-5d8dde16dc3c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="67738394-1d8a-43c4-9891-d7e1fdf7c6ea"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
-    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F035731F-8448-43E0-A923-EE7485D1B78B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8913,4 +8955,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25576F2-DA56-4DAD-9B77-0093008FA3D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rapport et Code final
Développement à 80% du retour d’expérience et correction et optimisation du code après l’auto-évaluation
</commit_message>
<xml_diff>
--- a/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
+++ b/Doc/P_Bulle_Snale-Toledo_Adran-jnltrav1.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="70">
   <si>
     <t>Classe :</t>
   </si>
@@ -284,6 +284,20 @@
 Recréation du code sans utiliser les boucles while et for 
 Fonctionnement en mode pause 
 </t>
+  </si>
+  <si>
+    <t>Explication du code de Snake (pas terminé)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code expliqué avec commentaires
+Respecter les règles du projet :
+    - Récupérer des classes dans des fichiers externes
+    - Utilisation de fonctions avec des flèches
+     - Boucles de style Java Script
+     - Utilisation du reste dans les tableaux.  </t>
+  </si>
+  <si>
+    <t>Recherche de problèmes et de solutions</t>
   </si>
 </sst>
 </file>
@@ -1393,11 +1407,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1408,12 +1432,6 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1422,10 +1440,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2294,10 +2308,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="116"/>
+      <c r="C19" s="117"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3143,27 +3157,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3193,27 +3207,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3249,146 +3263,146 @@
       <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="117" t="s">
+      <c r="D2" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="119"/>
-      <c r="S2" s="117" t="s">
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
-      <c r="AA2" s="118"/>
-      <c r="AB2" s="118"/>
-      <c r="AC2" s="118"/>
-      <c r="AD2" s="118"/>
-      <c r="AE2" s="118"/>
-      <c r="AF2" s="118"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="117" t="s">
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="118"/>
-      <c r="AJ2" s="118"/>
-      <c r="AK2" s="118"/>
-      <c r="AL2" s="118"/>
-      <c r="AM2" s="118"/>
-      <c r="AN2" s="118"/>
-      <c r="AO2" s="118"/>
-      <c r="AP2" s="118"/>
-      <c r="AQ2" s="118"/>
-      <c r="AR2" s="118"/>
-      <c r="AS2" s="118"/>
-      <c r="AT2" s="118"/>
-      <c r="AU2" s="118"/>
-      <c r="AV2" s="119"/>
-      <c r="AW2" s="117" t="s">
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="121"/>
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="121"/>
+      <c r="AT2" s="121"/>
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="122"/>
+      <c r="AW2" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="118"/>
-      <c r="AY2" s="118"/>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="118"/>
-      <c r="BD2" s="118"/>
-      <c r="BE2" s="118"/>
-      <c r="BF2" s="118"/>
-      <c r="BG2" s="118"/>
-      <c r="BH2" s="118"/>
-      <c r="BI2" s="118"/>
-      <c r="BJ2" s="118"/>
-      <c r="BK2" s="119"/>
-      <c r="BL2" s="117" t="s">
+      <c r="AX2" s="121"/>
+      <c r="AY2" s="121"/>
+      <c r="AZ2" s="121"/>
+      <c r="BA2" s="121"/>
+      <c r="BB2" s="121"/>
+      <c r="BC2" s="121"/>
+      <c r="BD2" s="121"/>
+      <c r="BE2" s="121"/>
+      <c r="BF2" s="121"/>
+      <c r="BG2" s="121"/>
+      <c r="BH2" s="121"/>
+      <c r="BI2" s="121"/>
+      <c r="BJ2" s="121"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="BM2" s="118"/>
-      <c r="BN2" s="118"/>
-      <c r="BO2" s="118"/>
-      <c r="BP2" s="118"/>
-      <c r="BQ2" s="118"/>
-      <c r="BR2" s="118"/>
-      <c r="BS2" s="118"/>
-      <c r="BT2" s="118"/>
-      <c r="BU2" s="118"/>
-      <c r="BV2" s="118"/>
-      <c r="BW2" s="118"/>
-      <c r="BX2" s="118"/>
-      <c r="BY2" s="118"/>
-      <c r="BZ2" s="119"/>
-      <c r="CA2" s="117" t="s">
+      <c r="BM2" s="121"/>
+      <c r="BN2" s="121"/>
+      <c r="BO2" s="121"/>
+      <c r="BP2" s="121"/>
+      <c r="BQ2" s="121"/>
+      <c r="BR2" s="121"/>
+      <c r="BS2" s="121"/>
+      <c r="BT2" s="121"/>
+      <c r="BU2" s="121"/>
+      <c r="BV2" s="121"/>
+      <c r="BW2" s="121"/>
+      <c r="BX2" s="121"/>
+      <c r="BY2" s="121"/>
+      <c r="BZ2" s="122"/>
+      <c r="CA2" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="CB2" s="118"/>
-      <c r="CC2" s="118"/>
-      <c r="CD2" s="118"/>
-      <c r="CE2" s="118"/>
-      <c r="CF2" s="118"/>
-      <c r="CG2" s="118"/>
-      <c r="CH2" s="118"/>
-      <c r="CI2" s="118"/>
-      <c r="CJ2" s="118"/>
-      <c r="CK2" s="118"/>
-      <c r="CL2" s="118"/>
-      <c r="CM2" s="118"/>
-      <c r="CN2" s="118"/>
-      <c r="CO2" s="119"/>
-      <c r="CP2" s="117" t="s">
+      <c r="CB2" s="121"/>
+      <c r="CC2" s="121"/>
+      <c r="CD2" s="121"/>
+      <c r="CE2" s="121"/>
+      <c r="CF2" s="121"/>
+      <c r="CG2" s="121"/>
+      <c r="CH2" s="121"/>
+      <c r="CI2" s="121"/>
+      <c r="CJ2" s="121"/>
+      <c r="CK2" s="121"/>
+      <c r="CL2" s="121"/>
+      <c r="CM2" s="121"/>
+      <c r="CN2" s="121"/>
+      <c r="CO2" s="122"/>
+      <c r="CP2" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="CQ2" s="118"/>
-      <c r="CR2" s="118"/>
-      <c r="CS2" s="118"/>
-      <c r="CT2" s="118"/>
-      <c r="CU2" s="118"/>
-      <c r="CV2" s="118"/>
-      <c r="CW2" s="118"/>
-      <c r="CX2" s="118"/>
-      <c r="CY2" s="118"/>
-      <c r="CZ2" s="118"/>
-      <c r="DA2" s="118"/>
-      <c r="DB2" s="118"/>
-      <c r="DC2" s="118"/>
-      <c r="DD2" s="119"/>
-      <c r="DE2" s="117" t="s">
+      <c r="CQ2" s="121"/>
+      <c r="CR2" s="121"/>
+      <c r="CS2" s="121"/>
+      <c r="CT2" s="121"/>
+      <c r="CU2" s="121"/>
+      <c r="CV2" s="121"/>
+      <c r="CW2" s="121"/>
+      <c r="CX2" s="121"/>
+      <c r="CY2" s="121"/>
+      <c r="CZ2" s="121"/>
+      <c r="DA2" s="121"/>
+      <c r="DB2" s="121"/>
+      <c r="DC2" s="121"/>
+      <c r="DD2" s="122"/>
+      <c r="DE2" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="DF2" s="118"/>
-      <c r="DG2" s="118"/>
-      <c r="DH2" s="118"/>
-      <c r="DI2" s="118"/>
-      <c r="DJ2" s="118"/>
-      <c r="DK2" s="118"/>
-      <c r="DL2" s="118"/>
-      <c r="DM2" s="118"/>
-      <c r="DN2" s="118"/>
-      <c r="DO2" s="118"/>
-      <c r="DP2" s="118"/>
-      <c r="DQ2" s="118"/>
-      <c r="DR2" s="118"/>
-      <c r="DS2" s="119"/>
+      <c r="DF2" s="121"/>
+      <c r="DG2" s="121"/>
+      <c r="DH2" s="121"/>
+      <c r="DI2" s="121"/>
+      <c r="DJ2" s="121"/>
+      <c r="DK2" s="121"/>
+      <c r="DL2" s="121"/>
+      <c r="DM2" s="121"/>
+      <c r="DN2" s="121"/>
+      <c r="DO2" s="121"/>
+      <c r="DP2" s="121"/>
+      <c r="DQ2" s="121"/>
+      <c r="DR2" s="121"/>
+      <c r="DS2" s="122"/>
     </row>
     <row r="3" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90"/>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="123" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="16">
@@ -3517,7 +3531,7 @@
     </row>
     <row r="4" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="90"/>
-      <c r="B4" s="123"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3643,7 +3657,7 @@
       <c r="DS4" s="100"/>
     </row>
     <row r="5" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="str">
+      <c r="B5" s="125" t="str">
         <f>Donnees!$C$21</f>
         <v>Rédaction JNLTRAV</v>
       </c>
@@ -3772,7 +3786,7 @@
       <c r="DS5" s="95"/>
     </row>
     <row r="6" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="121"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="102">
         <v>0</v>
       </c>
@@ -3898,7 +3912,7 @@
       <c r="DS6" s="100"/>
     </row>
     <row r="7" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="120" t="str">
+      <c r="B7" s="118" t="str">
         <f>Donnees!$C$22</f>
         <v>Vacances</v>
       </c>
@@ -4027,7 +4041,7 @@
       <c r="DS7" s="95"/>
     </row>
     <row r="8" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="121"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="102">
         <v>0</v>
       </c>
@@ -4153,7 +4167,7 @@
       <c r="DS8" s="100"/>
     </row>
     <row r="9" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="120" t="str">
+      <c r="B9" s="118" t="str">
         <f>Donnees!$C$23</f>
         <v>Absent</v>
       </c>
@@ -4282,7 +4296,7 @@
       <c r="DS9" s="95"/>
     </row>
     <row r="10" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="121"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="102">
         <v>0</v>
       </c>
@@ -4408,7 +4422,7 @@
       <c r="DS10" s="100"/>
     </row>
     <row r="11" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="120" t="str">
+      <c r="B11" s="118" t="str">
         <f>Donnees!$C$24</f>
         <v>Autres</v>
       </c>
@@ -4537,7 +4551,7 @@
       <c r="DS11" s="95"/>
     </row>
     <row r="12" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="121"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="102">
         <v>0</v>
       </c>
@@ -4663,7 +4677,7 @@
       <c r="DS12" s="100"/>
     </row>
     <row r="13" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="120" t="str">
+      <c r="B13" s="118" t="str">
         <f>Donnees!$C$25</f>
         <v>P_B : code</v>
       </c>
@@ -4792,7 +4806,7 @@
       <c r="DS13" s="95"/>
     </row>
     <row r="14" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="121"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="102">
         <v>0</v>
       </c>
@@ -4918,7 +4932,7 @@
       <c r="DS14" s="100"/>
     </row>
     <row r="15" spans="1:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="120" t="str">
+      <c r="B15" s="118" t="str">
         <f>Donnees!$C$26</f>
         <v xml:space="preserve">P_B : support de cours </v>
       </c>
@@ -5048,7 +5062,7 @@
     </row>
     <row r="16" spans="1:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="103"/>
-      <c r="B16" s="121"/>
+      <c r="B16" s="119"/>
       <c r="C16" s="102">
         <v>0</v>
       </c>
@@ -5174,7 +5188,7 @@
       <c r="DS16" s="100"/>
     </row>
     <row r="17" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="120" t="str">
+      <c r="B17" s="118" t="str">
         <f>Donnees!$C$27</f>
         <v>Livraison</v>
       </c>
@@ -5303,7 +5317,7 @@
       <c r="DS17" s="95"/>
     </row>
     <row r="18" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="121"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="102">
         <v>0</v>
       </c>
@@ -5429,7 +5443,7 @@
       <c r="DS18" s="100"/>
     </row>
     <row r="19" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="120" t="str">
+      <c r="B19" s="118" t="str">
         <f>Donnees!$C$28</f>
         <v>JavaScriptInfo</v>
       </c>
@@ -5558,7 +5572,7 @@
       <c r="DS19" s="95"/>
     </row>
     <row r="20" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="121"/>
+      <c r="B20" s="119"/>
       <c r="C20" s="102">
         <v>0</v>
       </c>
@@ -5684,7 +5698,7 @@
       <c r="DS20" s="100"/>
     </row>
     <row r="21" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="120" t="str">
+      <c r="B21" s="118" t="str">
         <f>Donnees!$C$29</f>
         <v>Test</v>
       </c>
@@ -5813,7 +5827,7 @@
       <c r="DS21" s="95"/>
     </row>
     <row r="22" spans="2:123" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="121"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="102">
         <v>0</v>
       </c>
@@ -5939,7 +5953,7 @@
       <c r="DS22" s="100"/>
     </row>
     <row r="23" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="120" t="str">
+      <c r="B23" s="118" t="str">
         <f>Donnees!$C$30</f>
         <v>Présentation du corus</v>
       </c>
@@ -6068,7 +6082,7 @@
       <c r="DS23" s="95"/>
     </row>
     <row r="24" spans="2:123" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="121"/>
+      <c r="B24" s="119"/>
       <c r="C24" s="102">
         <v>0</v>
       </c>
@@ -6454,6 +6468,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="DE2:DS2"/>
+    <mergeCell ref="S2:AG2"/>
+    <mergeCell ref="AH2:AV2"/>
+    <mergeCell ref="AW2:BK2"/>
+    <mergeCell ref="BL2:BZ2"/>
+    <mergeCell ref="CA2:CO2"/>
+    <mergeCell ref="CP2:DD2"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D2:R2"/>
@@ -6461,18 +6487,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="DE2:DS2"/>
-    <mergeCell ref="S2:AG2"/>
-    <mergeCell ref="AH2:AV2"/>
-    <mergeCell ref="AW2:BK2"/>
-    <mergeCell ref="BL2:BZ2"/>
-    <mergeCell ref="CA2:CO2"/>
-    <mergeCell ref="CP2:DD2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="DureeTropLongue" error="Cette durée est invalide: ce n'est pas un chiffre entier positif ou elle dépasse la &quot;Durée totale&quot; définie plus haut ..." sqref="C25">
@@ -6516,7 +6530,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="123" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="16">
@@ -6525,7 +6539,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="125"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -7328,8 +7342,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8093,7 +8107,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="54" x14ac:dyDescent="0.25">
-      <c r="A79" s="126" t="s">
+      <c r="A79" s="115" t="s">
         <v>40</v>
       </c>
       <c r="B79" s="4">
@@ -8255,27 +8269,51 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="9"/>
+      <c r="A98" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" s="4">
+        <v>1</v>
+      </c>
+      <c r="C98" s="112" t="s">
+        <v>54</v>
+      </c>
       <c r="D98" s="9"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="10"/>
+    <row r="99" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B99" s="2">
+        <v>6</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="10"/>
+      <c r="A100" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="10"/>
+    <row r="101" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B101" s="2">
+        <v>6</v>
+      </c>
+      <c r="C101" s="113" t="s">
+        <v>68</v>
+      </c>
       <c r="D101" s="10"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -8350,7 +8388,7 @@
       </c>
       <c r="B113" s="48">
         <f>SUM(B98:B112)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C113" s="111" t="s">
         <v>45</v>
@@ -8702,6 +8740,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4cb0ad740d14d835234d40feeeca33f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8afc1019b1abb7dd8f9636ee686097" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -8918,27 +8976,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25576F2-DA56-4DAD-9B77-0093008FA3D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98d92101-24da-4498-9971-a24673344bd8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F035731F-8448-43E0-A923-EE7485D1B78B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8955,29 +9018,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A79CA8D3-86C8-4C18-8AF8-8AB81EA18092}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25576F2-DA56-4DAD-9B77-0093008FA3D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
-    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>